<commit_message>
Updated power budget with new peak and average tables
</commit_message>
<xml_diff>
--- a/Sheets/Power Budget.xlsx
+++ b/Sheets/Power Budget.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zack/Documents/Stanford/AA236/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF5A68B-7ACF-9346-9146-B62C63BAC64E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
   <si>
     <t>Item</t>
   </si>
@@ -69,13 +75,28 @@
   </si>
   <si>
     <t>Totals</t>
+  </si>
+  <si>
+    <t>Nichrome burn wire</t>
+  </si>
+  <si>
+    <t>Deployment and Detumble Operations</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Peak</t>
+  </si>
+  <si>
+    <t>Nominal Operations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +112,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -100,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -117,11 +153,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -138,10 +183,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -153,6 +229,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -420,14 +499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -436,7 +515,7 @@
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="34">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -478,7 +557,7 @@
         <v>6.12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -492,15 +571,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E8" si="0">B3*D3</f>
+        <f t="shared" ref="E3:E9" si="0">B3*D3</f>
         <v>1019.9999999999999</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F8" si="1">C3*D3</f>
+        <f t="shared" ref="F3:F9" si="1">C3*D3</f>
         <v>5100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -522,7 +601,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -544,7 +623,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -566,7 +645,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -588,46 +667,594 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:6" ht="17">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="7">
         <v>3.11</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>3.11</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <v>1.8</v>
       </c>
-      <c r="E8" s="6">
-        <f t="shared" si="0"/>
+      <c r="E8" s="7">
+        <f>B8*D8</f>
         <v>5.5979999999999999</v>
       </c>
-      <c r="F8" s="6">
-        <f t="shared" si="1"/>
+      <c r="F8" s="7">
+        <f>C8*D8</f>
         <v>5.5979999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:6" ht="17">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1700</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1700</v>
+      </c>
+      <c r="D9" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="E9" s="6">
+        <f>B9*D9</f>
+        <v>5610</v>
+      </c>
+      <c r="F9" s="6">
+        <f>C9*D9</f>
+        <v>5610</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
-        <f>SUM(B2:B8)</f>
+      <c r="B10" s="10">
+        <f>SUM(B2:B9)</f>
+        <v>2285.21</v>
+      </c>
+      <c r="C10" s="10">
+        <f>SUM(C2:C9)</f>
+        <v>3826.51</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10">
+        <f>SUM(E2:E9)</f>
+        <v>8280.9779999999992</v>
+      </c>
+      <c r="F10" s="10">
+        <f>SUM(F2:F9)</f>
+        <v>14209.717999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="34">
+      <c r="B17" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="1:7" ht="17">
+      <c r="B18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="E18" s="12">
+        <f>C18*D18</f>
+        <v>1.9800000000000002</v>
+      </c>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" ht="17">
+      <c r="B19" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="12">
+        <v>16</v>
+      </c>
+      <c r="D19" s="12">
+        <v>2.4</v>
+      </c>
+      <c r="E19" s="12">
+        <f t="shared" ref="E19:E21" si="2">C19*D19</f>
+        <v>38.4</v>
+      </c>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:7" ht="17">
+      <c r="B20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="13">
+        <v>35</v>
+      </c>
+      <c r="D20" s="12">
+        <v>5</v>
+      </c>
+      <c r="E20" s="12">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:7" ht="17">
+      <c r="B21" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="12">
+        <v>3.11</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="E21" s="12">
+        <f t="shared" si="2"/>
+        <v>5.5979999999999999</v>
+      </c>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:7" ht="17">
+      <c r="B22" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="15">
+        <f>SUM(C18:C21)</f>
+        <v>55.21</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15">
+        <f>SUM(E18:E21)</f>
+        <v>220.97800000000001</v>
+      </c>
+      <c r="G22" s="19"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" ht="17">
+      <c r="A24" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" ht="34">
+      <c r="B25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="20"/>
+    </row>
+    <row r="26" spans="1:7" ht="17">
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="E26" s="2">
+        <f>C26*D26</f>
+        <v>6.12</v>
+      </c>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" ht="17">
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>130</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="E27" s="2">
+        <f>C27*D27</f>
+        <v>312</v>
+      </c>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" ht="17">
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="3">
+        <v>240</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2">
+        <f>C28*D28</f>
+        <v>1200</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="17">
+      <c r="B29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="7">
+        <v>3.11</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="E29" s="7">
+        <f>C29*D29</f>
+        <v>5.5979999999999999</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="17">
+      <c r="B30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1700</v>
+      </c>
+      <c r="D30" s="6">
+        <v>3.3</v>
+      </c>
+      <c r="E30" s="6">
+        <f>C30*D30</f>
+        <v>5610</v>
+      </c>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" ht="17">
+      <c r="B31" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="10">
+        <f>SUM(C26:C30)</f>
+        <v>2076.5100000000002</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10">
+        <f>SUM(E26:E30)</f>
+        <v>7133.7179999999998</v>
+      </c>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" ht="34">
+      <c r="B36" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="1:8" ht="17">
+      <c r="B37" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D37" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="E37" s="12">
+        <v>1.98</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="1:8" ht="17">
+      <c r="B38" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="12">
+        <v>200</v>
+      </c>
+      <c r="D38" s="12">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E38" s="12">
+        <v>1020</v>
+      </c>
+      <c r="F38" s="8"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" ht="17">
+      <c r="B39" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="12">
+        <v>200</v>
+      </c>
+      <c r="D39" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="E39" s="12">
+        <v>260</v>
+      </c>
+      <c r="F39" s="8"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="1:8" ht="17">
+      <c r="B40" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="12">
+        <v>16</v>
+      </c>
+      <c r="D40" s="12">
+        <v>2.4</v>
+      </c>
+      <c r="E40" s="12">
+        <v>38.4</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="1:8" ht="17">
+      <c r="B41" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="13">
+        <v>35</v>
+      </c>
+      <c r="D41" s="12">
+        <v>5</v>
+      </c>
+      <c r="E41" s="12">
+        <v>175</v>
+      </c>
+      <c r="F41" s="8"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="8"/>
+    </row>
+    <row r="42" spans="1:8" ht="17">
+      <c r="B42" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="12">
+        <v>130</v>
+      </c>
+      <c r="D42" s="12">
+        <v>9</v>
+      </c>
+      <c r="E42" s="12">
+        <v>1170</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="1:8" ht="17">
+      <c r="B43" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="12">
+        <v>3.11</v>
+      </c>
+      <c r="D43" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="E43" s="12">
+        <v>5.5979999999999999</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="1:8" ht="17">
+      <c r="B44" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="15">
+        <f>SUM(C37:C43)</f>
         <v>585.21</v>
       </c>
-      <c r="C9">
-        <f t="shared" ref="C9:F9" si="2">SUM(C2:C8)</f>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15">
+        <f>SUM(E37:E43)</f>
+        <v>2670.9780000000001</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="34">
+      <c r="B47" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="17">
+      <c r="B48" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="12">
+        <v>3.4</v>
+      </c>
+      <c r="D48" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="E48" s="12">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="17">
+      <c r="B49" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="12">
+        <v>1000</v>
+      </c>
+      <c r="D49" s="12">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E49" s="12">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="17">
+      <c r="B50" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="12">
+        <v>620</v>
+      </c>
+      <c r="D50" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="E50" s="12">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="17">
+      <c r="B51" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="12">
+        <v>130</v>
+      </c>
+      <c r="D51" s="12">
+        <v>2.4</v>
+      </c>
+      <c r="E51" s="12">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="17">
+      <c r="B52" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="13">
+        <v>240</v>
+      </c>
+      <c r="D52" s="12">
+        <v>5</v>
+      </c>
+      <c r="E52" s="12">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="17">
+      <c r="B53" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="12">
+        <v>130</v>
+      </c>
+      <c r="D53" s="12">
+        <v>9</v>
+      </c>
+      <c r="E53" s="12">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="17">
+      <c r="B54" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="12">
+        <v>3.11</v>
+      </c>
+      <c r="D54" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="E54" s="12">
+        <v>5.5979999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="17">
+      <c r="B55" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="15">
+        <f>SUM(C48:C54)</f>
         <v>2126.5100000000002</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>2670.9780000000001</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15">
+        <f>SUM(E48:E54)</f>
         <v>8599.7179999999989</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated with margin calculations
</commit_message>
<xml_diff>
--- a/Sheets/Power Budget.xlsx
+++ b/Sheets/Power Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Zack/Documents/Stanford/AA236/Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF5A68B-7ACF-9346-9146-B62C63BAC64E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7E0F80-7AED-7B47-B9AB-DC61B93CA447}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="21">
   <si>
     <t>Item</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Nominal Operations</t>
+  </si>
+  <si>
+    <t>Margin (%)</t>
+  </si>
+  <si>
+    <t>Margin</t>
   </si>
 </sst>
 </file>
@@ -166,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -206,7 +212,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -220,6 +225,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -535,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="17">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -557,7 +564,7 @@
         <v>6.12</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="17">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -571,15 +578,15 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E9" si="0">B3*D3</f>
+        <f t="shared" ref="E3:E7" si="0">B3*D3</f>
         <v>1019.9999999999999</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F9" si="1">C3*D3</f>
+        <f t="shared" ref="F3:F7" si="1">C3*D3</f>
         <v>5100</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="17">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -601,7 +608,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="17">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -623,7 +630,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="17">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -645,7 +652,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="17">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -711,7 +718,7 @@
         <v>5610</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="17">
       <c r="A10" s="9" t="s">
         <v>13</v>
       </c>
@@ -756,7 +763,7 @@
       <c r="E17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="17"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:7" ht="17">
       <c r="B18" s="12" t="s">
@@ -772,7 +779,7 @@
         <f>C18*D18</f>
         <v>1.9800000000000002</v>
       </c>
-      <c r="G18" s="18"/>
+      <c r="G18" s="17"/>
     </row>
     <row r="19" spans="1:7" ht="17">
       <c r="B19" s="12" t="s">
@@ -788,7 +795,7 @@
         <f t="shared" ref="E19:E21" si="2">C19*D19</f>
         <v>38.4</v>
       </c>
-      <c r="G19" s="18"/>
+      <c r="G19" s="17"/>
     </row>
     <row r="20" spans="1:7" ht="17">
       <c r="B20" s="12" t="s">
@@ -804,7 +811,7 @@
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
-      <c r="G20" s="18"/>
+      <c r="G20" s="17"/>
     </row>
     <row r="21" spans="1:7" ht="17">
       <c r="B21" s="12" t="s">
@@ -820,443 +827,546 @@
         <f t="shared" si="2"/>
         <v>5.5979999999999999</v>
       </c>
-      <c r="G21" s="18"/>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="1:7" ht="17">
       <c r="B22" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="15">
-        <f>SUM(C18:C21)</f>
+      <c r="C22" s="20">
+        <f>SUM(C15:C21)</f>
         <v>55.21</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15">
-        <f>SUM(E18:E21)</f>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20">
+        <f>SUM(E15:E21)</f>
         <v>220.97800000000001</v>
       </c>
-      <c r="G22" s="19"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="G23" s="8"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" ht="17">
+      <c r="B23" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="21">
+        <f>5200-C22</f>
+        <v>5144.79</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21">
+        <f>2470-E22</f>
+        <v>2249.0219999999999</v>
+      </c>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" ht="17">
-      <c r="A24" s="16" t="s">
+      <c r="B24" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="21">
+        <f>C23/5200*100</f>
+        <v>98.938269230769222</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21">
+        <f>E23/2470*100</f>
+        <v>91.053522267206475</v>
+      </c>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" ht="17">
+      <c r="A26" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" ht="34">
-      <c r="B25" s="1" t="s">
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" ht="34">
+      <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" ht="17">
-      <c r="B26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2">
-        <v>3.4</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="E26" s="2">
-        <f>C26*D26</f>
-        <v>6.12</v>
-      </c>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" ht="17">
-      <c r="B27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="2">
-        <v>130</v>
-      </c>
-      <c r="D27" s="2">
-        <v>2.4</v>
-      </c>
-      <c r="E27" s="2">
-        <f>C27*D27</f>
-        <v>312</v>
-      </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:7" ht="17">
       <c r="B28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="3">
-        <v>240</v>
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>3.4</v>
       </c>
       <c r="D28" s="2">
-        <v>5</v>
+        <v>1.8</v>
       </c>
       <c r="E28" s="2">
         <f>C28*D28</f>
+        <v>6.12</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" ht="17">
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>130</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="E29" s="2">
+        <f>C29*D29</f>
+        <v>312</v>
+      </c>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="17">
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="3">
+        <v>240</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <f>C30*D30</f>
         <v>1200</v>
       </c>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" ht="17">
-      <c r="B29" s="7" t="s">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" ht="17">
+      <c r="B31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C31" s="7">
         <v>3.11</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D31" s="7">
         <v>1.8</v>
       </c>
-      <c r="E29" s="7">
-        <f>C29*D29</f>
+      <c r="E31" s="7">
+        <f>C31*D31</f>
         <v>5.5979999999999999</v>
       </c>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" ht="17">
-      <c r="B30" s="6" t="s">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" ht="17">
+      <c r="B32" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C32" s="6">
         <v>1700</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D32" s="6">
         <v>3.3</v>
       </c>
-      <c r="E30" s="6">
-        <f>C30*D30</f>
+      <c r="E32" s="6">
+        <f>C32*D32</f>
         <v>5610</v>
       </c>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" ht="17">
-      <c r="B31" s="9" t="s">
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" ht="17">
+      <c r="B33" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="10">
-        <f>SUM(C26:C30)</f>
+      <c r="C33" s="20">
+        <f>SUM(C26:C32)</f>
         <v>2076.5100000000002</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10">
-        <f>SUM(E26:E30)</f>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20">
+        <f>SUM(E26:E32)</f>
         <v>7133.7179999999998</v>
       </c>
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:8">
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
+    <row r="34" spans="1:8" ht="17">
+      <c r="B34" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="21">
+        <f>5200-C33</f>
+        <v>3123.49</v>
+      </c>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21">
+        <f>2470-E33</f>
+        <v>-4663.7179999999998</v>
+      </c>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="1:8" ht="17">
+      <c r="B35" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="21">
+        <f>C34/5200*100</f>
+        <v>60.067115384615377</v>
+      </c>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21">
+        <f>E34/2470*100</f>
+        <v>-188.81449392712551</v>
+      </c>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:8" ht="34">
-      <c r="B36" s="11" t="s">
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:8" ht="34">
+      <c r="B40" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C40" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E40" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" ht="17">
-      <c r="B37" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D37" s="12">
-        <v>1.8</v>
-      </c>
-      <c r="E37" s="12">
-        <v>1.98</v>
-      </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="1:8" ht="17">
-      <c r="B38" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="12">
-        <v>200</v>
-      </c>
-      <c r="D38" s="12">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E38" s="12">
-        <v>1020</v>
-      </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8" ht="17">
-      <c r="B39" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C39" s="12">
-        <v>200</v>
-      </c>
-      <c r="D39" s="12">
-        <v>1.3</v>
-      </c>
-      <c r="E39" s="12">
-        <v>260</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="8"/>
-    </row>
-    <row r="40" spans="1:8" ht="17">
-      <c r="B40" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="12">
-        <v>16</v>
-      </c>
-      <c r="D40" s="12">
-        <v>2.4</v>
-      </c>
-      <c r="E40" s="12">
-        <v>38.4</v>
-      </c>
       <c r="F40" s="8"/>
-      <c r="G40" s="18"/>
+      <c r="G40" s="16"/>
       <c r="H40" s="8"/>
     </row>
     <row r="41" spans="1:8" ht="17">
       <c r="B41" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="13">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="C41" s="12">
+        <v>1.1000000000000001</v>
       </c>
       <c r="D41" s="12">
-        <v>5</v>
+        <v>1.8</v>
       </c>
       <c r="E41" s="12">
-        <v>175</v>
+        <v>1.98</v>
       </c>
       <c r="F41" s="8"/>
-      <c r="G41" s="18"/>
+      <c r="G41" s="17"/>
       <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" ht="17">
       <c r="B42" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C42" s="12">
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="D42" s="12">
-        <v>9</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E42" s="12">
-        <v>1170</v>
+        <v>1020</v>
       </c>
       <c r="F42" s="8"/>
-      <c r="G42" s="18"/>
+      <c r="G42" s="17"/>
       <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" ht="17">
       <c r="B43" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="12">
+        <v>200</v>
+      </c>
+      <c r="D43" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="E43" s="12">
+        <v>260</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="1:8" ht="17">
+      <c r="B44" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="12">
+        <v>16</v>
+      </c>
+      <c r="D44" s="12">
+        <v>2.4</v>
+      </c>
+      <c r="E44" s="12">
+        <v>38.4</v>
+      </c>
+      <c r="F44" s="8"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="1:8" ht="17">
+      <c r="B45" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="13">
+        <v>35</v>
+      </c>
+      <c r="D45" s="12">
+        <v>5</v>
+      </c>
+      <c r="E45" s="12">
+        <v>175</v>
+      </c>
+      <c r="F45" s="8"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="1:8" ht="17">
+      <c r="B46" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C46" s="12">
         <v>3.11</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D46" s="12">
         <v>1.8</v>
       </c>
-      <c r="E43" s="12">
+      <c r="E46" s="12">
         <v>5.5979999999999999</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="8"/>
-    </row>
-    <row r="44" spans="1:8" ht="17">
-      <c r="B44" s="14" t="s">
+      <c r="F46" s="8"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="1:8" ht="17">
+      <c r="B47" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="15">
-        <f>SUM(C37:C43)</f>
-        <v>585.21</v>
-      </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15">
-        <f>SUM(E37:E43)</f>
-        <v>2670.9780000000001</v>
-      </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="8"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
+      <c r="C47" s="20">
+        <f>SUM(C40:C46)</f>
+        <v>455.21000000000004</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20">
+        <f>SUM(E40:E46)</f>
+        <v>1500.9780000000001</v>
+      </c>
+      <c r="F47" s="8"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" ht="17">
+      <c r="B48" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="21">
+        <f>5200-C47</f>
+        <v>4744.79</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21">
+        <f>2470-E47</f>
+        <v>969.02199999999993</v>
+      </c>
+      <c r="G48" s="18"/>
+    </row>
+    <row r="49" spans="1:7" ht="17">
+      <c r="B49" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="21">
+        <f>C48/5200*100</f>
+        <v>91.245961538461543</v>
+      </c>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21">
+        <f>E48/2470*100</f>
+        <v>39.231659919028338</v>
+      </c>
+      <c r="G49" s="18"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="34">
-      <c r="B47" s="11" t="s">
+    <row r="52" spans="1:7" ht="34">
+      <c r="B52" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C52" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E52" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="17">
-      <c r="B48" s="12" t="s">
+    <row r="53" spans="1:7" ht="17">
+      <c r="B53" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C53" s="12">
         <v>3.4</v>
       </c>
-      <c r="D48" s="12">
+      <c r="D53" s="12">
         <v>1.8</v>
       </c>
-      <c r="E48" s="12">
+      <c r="E53" s="12">
         <v>6.12</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="17">
-      <c r="B49" s="12" t="s">
+    <row r="54" spans="1:7" ht="17">
+      <c r="B54" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="12">
+      <c r="C54" s="12">
         <v>1000</v>
       </c>
-      <c r="D49" s="12">
+      <c r="D54" s="12">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E49" s="12">
+      <c r="E54" s="12">
         <v>5100</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="17">
-      <c r="B50" s="12" t="s">
+    <row r="55" spans="1:7" ht="17">
+      <c r="B55" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C50" s="12">
+      <c r="C55" s="12">
         <v>620</v>
       </c>
-      <c r="D50" s="12">
+      <c r="D55" s="12">
         <v>1.3</v>
       </c>
-      <c r="E50" s="12">
+      <c r="E55" s="12">
         <v>806</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="17">
-      <c r="B51" s="12" t="s">
+    <row r="56" spans="1:7" ht="17">
+      <c r="B56" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="12">
+      <c r="C56" s="12">
         <v>130</v>
       </c>
-      <c r="D51" s="12">
+      <c r="D56" s="12">
         <v>2.4</v>
       </c>
-      <c r="E51" s="12">
+      <c r="E56" s="12">
         <v>312</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="17">
-      <c r="B52" s="12" t="s">
+    <row r="57" spans="1:7" ht="17">
+      <c r="B57" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="13">
+      <c r="C57" s="13">
         <v>240</v>
       </c>
-      <c r="D52" s="12">
+      <c r="D57" s="12">
         <v>5</v>
       </c>
-      <c r="E52" s="12">
+      <c r="E57" s="12">
         <v>1200</v>
       </c>
     </row>
-    <row r="53" spans="2:5" ht="17">
-      <c r="B53" s="12" t="s">
+    <row r="58" spans="1:7" ht="17">
+      <c r="B58" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="12">
+      <c r="C58" s="12">
         <v>130</v>
       </c>
-      <c r="D53" s="12">
+      <c r="D58" s="12">
         <v>9</v>
       </c>
-      <c r="E53" s="12">
+      <c r="E58" s="12">
         <v>1170</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="17">
-      <c r="B54" s="12" t="s">
+    <row r="59" spans="1:7" ht="17">
+      <c r="B59" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="12">
+      <c r="C59" s="12">
         <v>3.11</v>
       </c>
-      <c r="D54" s="12">
+      <c r="D59" s="12">
         <v>1.8</v>
       </c>
-      <c r="E54" s="12">
+      <c r="E59" s="12">
         <v>5.5979999999999999</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="17">
-      <c r="B55" s="14" t="s">
+    <row r="60" spans="1:7" ht="17">
+      <c r="B60" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="15">
-        <f>SUM(C48:C54)</f>
+      <c r="C60" s="20">
+        <f>SUM(C53:C59)</f>
         <v>2126.5100000000002</v>
       </c>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15">
-        <f>SUM(E48:E54)</f>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20">
+        <f>SUM(E53:E59)</f>
         <v>8599.7179999999989</v>
       </c>
+    </row>
+    <row r="61" spans="1:7" ht="17">
+      <c r="B61" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="21">
+        <f>5200-C60</f>
+        <v>3073.49</v>
+      </c>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21">
+        <f>2470-E60</f>
+        <v>-6129.7179999999989</v>
+      </c>
+      <c r="G61" s="18"/>
+    </row>
+    <row r="62" spans="1:7" ht="17">
+      <c r="B62" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="21">
+        <f>C61/5200*100</f>
+        <v>59.105576923076917</v>
+      </c>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21">
+        <f>E61/2470*100</f>
+        <v>-248.16672064777325</v>
+      </c>
+      <c r="G62" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>